<commit_message>
makers name and designation in excel file created
</commit_message>
<xml_diff>
--- a/txxxxt/ProducthuntProduct.xlsx
+++ b/txxxxt/ProducthuntProduct.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\office\txxxxt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\office\scraping-data\txxxxt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="399">
   <si>
     <t>Id</t>
   </si>
@@ -36,6 +36,9 @@
     <t>Votescount</t>
   </si>
   <si>
+    <t>Makers Information</t>
+  </si>
+  <si>
     <t>Live Video Calling SDK by Dyte</t>
   </si>
   <si>
@@ -45,6 +48,17 @@
     <t>https://www.producthunt.com/posts/live-video-calling-sdk-by-dyte?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Live Video Calling SDK by Dyte
+January 2023
+Follow All
+Abhishek Kankani
+CEO &amp; Co-founder @Dyte
+Palash Golecha
+Co-founder dyte.io
+Kushagra Vaish
+Maker and reluctant leader</t>
+  </si>
+  <si>
     <t>LINER AI</t>
   </si>
   <si>
@@ -54,6 +68,79 @@
     <t>https://www.producthunt.com/posts/liner-ai?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>LINER AI
+January 2023
+Follow All
+Brian Woo
+Jinu Kim
+LINER CEO
+Youtube Highlighter by LINER
+August 2021
+Follow All
+Jinu Kim
+Improved Google Search by LINER
+December 2020
+Follow All
+Jinu Kim
+LINER CEO
+Brian Woo
+LINER Home
+August 2020
+Follow All
+Jinu Kim
+LINER CEO
+Brian Woo
+LINER Browser Extension
+August 2019
+Follow All
+Jinu Kim
+LINER CEO
+Brian Woo
+LINER 5
+August 2018
+Follow All
+Brian Woo
+Jinu Kim
+LINER CEO
+Highlighting API made by LINER
+November 2017
+Follow All
+Jinu Kim
+LINER CEO
+Sung Cho
+Brian Woo
+LINER for Safari
+May 2017
+Follow All
+Jinu Kim
+LINER CEO
+Sung Cho
+Brian Woo
+LINER for Pocket
+March 2017
+Follow All
+Min Park
+https://nexybit.com
+Jinu Kim
+LINER CEO
+Brian Woo
+LINER for iOS
+January 2017
+Follow All
+Min Park
+https://nexybit.com
+Jinu Kim
+LINER CEO
+Brian Woo
+Liner
+July 2015
+Follow All
+Brian Woo
+Jinu Kim
+LINER CEO
+Sung Cho</t>
+  </si>
+  <si>
     <t>Getgud.io</t>
   </si>
   <si>
@@ -63,6 +150,15 @@
     <t>https://www.producthunt.com/posts/getgud-io?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Getgud.io
+January 2023
+Follow All
+Art Kulakov
+ML Lead, B2B gaming startup founder
+guy kroupp
+Tech entrepreneur</t>
+  </si>
+  <si>
     <t>littlecook</t>
   </si>
   <si>
@@ -72,6 +168,15 @@
     <t>https://www.producthunt.com/posts/littlecook?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>littlecook
+January 2023
+Follow All
+Nimesh
+Founder littlecook.io ✦ ex-amazon
+Amir Andohkosh
+Founder</t>
+  </si>
+  <si>
     <t>Terrastruct</t>
   </si>
   <si>
@@ -81,6 +186,16 @@
     <t>https://www.producthunt.com/posts/terrastruct-3?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Terrastruct
+January 2023
+Follow All
+Alexander Wang
+Terrastruct
+January 2020
+Follow All
+Alexander Wang</t>
+  </si>
+  <si>
     <t>PriceWell Bubble Plugin for Stripe</t>
   </si>
   <si>
@@ -90,6 +205,15 @@
     <t>https://www.producthunt.com/posts/pricewell-bubble-plugin-for-stripe?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>PriceWell Bubble Plugin for Stripe
+January 2023
+Follow All
+Matthew Reid
+Co-Founder PriceWell.io
+Σπυρος Κοντοπριας
+A storyteller</t>
+  </si>
+  <si>
     <t>ChatGPT Famous Resumes</t>
   </si>
   <si>
@@ -99,6 +223,18 @@
     <t>https://www.producthunt.com/posts/chatgpt-famous-resumes?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>ChatGPT Famous Resumes
+January 2023
+Follow All
+Viktor Kirilov
+Software Engineer, Car Enthusiast
+This Resume Does Not Exist
+March 2019
+Follow All
+Viktor Kirilov
+Software Engineer, Car Enthusiast</t>
+  </si>
+  <si>
     <t>Delibr AI</t>
   </si>
   <si>
@@ -108,6 +244,32 @@
     <t>https://www.producthunt.com/posts/delibr-ai?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Delibr AI
+January 2023
+Follow All
+Nils Janse
+Founder of Delibr
+André Dantorp
+Startup and tech lover
+Fredrika Andersson
+Product designer @Delibr
+Erik Wenneborg
+Co founder at Delibr
+Farid Bonawiede
+Co founder at Delibr
+Nicole Landgraff
+Launching Delibr AI for Product Managers
+Delibr 2.0
+January 2022
+Follow All
+Nils Janse
+Founder of Delibr
+Farid Bonawiede
+Co founder at Delibr
+Erik Wenneborg
+Co founder at Delibr</t>
+  </si>
+  <si>
     <t>Kayyo</t>
   </si>
   <si>
@@ -117,6 +279,23 @@
     <t>https://www.producthunt.com/posts/kayyo?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Kayyo
+January 2023
+Follow All
+Labib Yasir
+Co-Founder &amp; CEO of Kayyo
+Ayman Saleh
+ML Engineer, Building perception systems
+tedjouc1
+Product Designer at Kayyo
+Mohamed Jaber
+iOS Software Engineer @ Kayyo
+Messipsa Tamazouzt
+software engineer
+Michael Paik
+Building Kayyo</t>
+  </si>
+  <si>
     <t>Femme Stock</t>
   </si>
   <si>
@@ -126,6 +305,13 @@
     <t>https://www.producthunt.com/posts/femme-stock?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Femme Stock
+January 2023
+Follow All
+Zeng
+Founder of FemmeStock &amp; WhoWhatWhyAi</t>
+  </si>
+  <si>
     <t>Zoom Timer BlueSky Apps</t>
   </si>
   <si>
@@ -135,6 +321,18 @@
     <t>https://www.producthunt.com/posts/zoom-timer-bluesky-apps?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Zoom Timer BlueSky Apps
+January 2023
+Follow All
+Ben Ross
+Mahin Ali
+SaaS Marketing
+BlueSky Timer for Zoom
+January 2022
+Follow All
+Ben Ross</t>
+  </si>
+  <si>
     <t>WhatsApp Beta</t>
   </si>
   <si>
@@ -144,6 +342,18 @@
     <t>https://www.producthunt.com/posts/whatsapp-beta?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Whatsapp Reminders
+June 2021
+Follow All
+Santhosh Kumar Elango
+Co-Founder and CEO at Leadfriday
+WhatsApp for Desktop
+June 2015
+Follow All
+Alexandru Rosianu
+Co-founder &amp; CTO @ Proptee</t>
+  </si>
+  <si>
     <t>balancez</t>
   </si>
   <si>
@@ -153,6 +363,13 @@
     <t>https://www.producthunt.com/posts/balancez?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>balancez
+January 2023
+Follow All
+Elif Duran
+Co-founder @BeforeSunset, learner&amp;maker</t>
+  </si>
+  <si>
     <t>Tibio</t>
   </si>
   <si>
@@ -162,6 +379,15 @@
     <t>https://www.producthunt.com/posts/tibio?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Tibio
+January 2023
+Follow All
+Patrik Svoboda
+Product designer, Tibio co-creator.
+Duc Phi Viet
+Hi, I am a creator of Tibio app.</t>
+  </si>
+  <si>
     <t>Monse</t>
   </si>
   <si>
@@ -171,6 +397,12 @@
     <t>https://www.producthunt.com/posts/monse-2?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Monse
+January 2023
+Follow All
+Víctor Falcón</t>
+  </si>
+  <si>
     <t>Nike Training Club on Netflix</t>
   </si>
   <si>
@@ -180,6 +412,17 @@
     <t>https://www.producthunt.com/posts/nike-training-club-on-netflix?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Interactive Storytelling from Netflix
+June 2017
+Follow All
+Dave Schlafman
+Netflix Offline
+November 2016
+Follow All
+Navin Iyengar
+Product Designer, Netflix</t>
+  </si>
+  <si>
     <t>bestcodingpractices.dev</t>
   </si>
   <si>
@@ -189,6 +432,24 @@
     <t>https://www.producthunt.com/posts/bestcodingpractices-dev?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>bestcodingpractices.dev
+January 2023
+Follow All
+Cédric Teyton
+CEO &amp; co-founder @Promyze
+Arthur Magne
+Co-founder &amp; CTO @ Promyze
+Xavier Blanc
+I am interested in software development
+Heloïse Birot
+https://promyze.com/
+Corentin Latappy
+Dev @Promyze
+Malo Couaran
+Budding software craftman
+Show all 7 makers</t>
+  </si>
+  <si>
     <t>Moonwalkers</t>
   </si>
   <si>
@@ -207,6 +468,19 @@
     <t>https://www.producthunt.com/posts/squaredance-for-shopify?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Squaredance for Shopify
+January 2023
+Follow All
+Shilpa Mandhan
+Head of Growth @ Squaredance
+Natalie Mastracci
+Product @ Squaredance
+Michael Fulton
+Growth Marketing Director
+Camay Lee
+Product marketer</t>
+  </si>
+  <si>
     <t>7-Day UX Job Hunting Challenge</t>
   </si>
   <si>
@@ -216,6 +490,32 @@
     <t>https://www.producthunt.com/posts/7-day-ux-job-hunting-challenge?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>7-Day UX Job Hunting Challenge
+January 2023
+Follow All
+Christopher Nguyen
+Making UX Playbook
+Bryant Castro
+Design leader growing teams &amp; products
+UX Interview Masterclass
+October 2022
+Follow All
+Christopher Nguyen
+Making UX Playbook
+Bryant Castro
+Design leader growing teams &amp; products
+UX Portfolio Playbook
+August 2022
+Follow All
+Christopher Nguyen
+Making UX Playbook
+UX Playbook 2.0
+May 2022
+Follow All
+Christopher Nguyen
+Making UX Playbook</t>
+  </si>
+  <si>
     <t>Whispr</t>
   </si>
   <si>
@@ -225,6 +525,13 @@
     <t>https://www.producthunt.com/posts/whispr-2?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Whispr
+January 2023
+Follow All
+Álvaro Pintado
+Co-Founder at Gox.</t>
+  </si>
+  <si>
     <t>This Product Does Not Exist</t>
   </si>
   <si>
@@ -234,6 +541,13 @@
     <t>https://www.producthunt.com/posts/this-product-does-not-exist-1?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>This Product Does Not Exist
+January 2023
+Follow All
+Mighil
+globe-earther and schnauzer enthusiast</t>
+  </si>
+  <si>
     <t>Fablegym</t>
   </si>
   <si>
@@ -243,6 +557,13 @@
     <t>https://www.producthunt.com/posts/fablegym?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Fablegym
+January 2023
+Follow All
+Solomon Kingsnorth
+Teacher</t>
+  </si>
+  <si>
     <t>ClipNinja</t>
   </si>
   <si>
@@ -252,6 +573,13 @@
     <t>https://www.producthunt.com/posts/clipninja-2?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>ClipNinja
+January 2023
+Follow All
+Libor Huspenina
+Apple platforms developer</t>
+  </si>
+  <si>
     <t>DeveloperHub.io</t>
   </si>
   <si>
@@ -261,6 +589,18 @@
     <t>https://www.producthunt.com/posts/developerhub-io-2?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>DeveloperHub.io
+January 2023
+Follow All
+Zaid Daba'een
+CEO &amp; Founder - DeveloperHub
+Developerhub.io
+July 2018
+Follow All
+Zaid Daba'een
+CEO &amp; Founder - DeveloperHub</t>
+  </si>
+  <si>
     <t>Qeraunos</t>
   </si>
   <si>
@@ -270,6 +610,17 @@
     <t>https://www.producthunt.com/posts/qeraunos?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Qeraunos
+January 2023
+Follow All
+Arthur Huynh
+Software Engineer at Qeraunos
+Dennis Cheung
+software engineer
+Amrit Ramos
+Software Engineer.</t>
+  </si>
+  <si>
     <t>Deploy Button for custom GPT-3 APIs</t>
   </si>
   <si>
@@ -279,6 +630,13 @@
     <t>https://www.producthunt.com/posts/deploy-button-for-custom-gpt-3-apis?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Deploy Button for custom GPT-3 APIs
+January 2023
+Follow All
+Ted Benson
+I turn research into product.</t>
+  </si>
+  <si>
     <t>Free Valentine's Day 3d illustrations</t>
   </si>
   <si>
@@ -288,6 +646,142 @@
     <t>https://www.producthunt.com/posts/free-valentine-s-day-3d-illustrations?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Free Valentine's Day 3d illustrations
+January 2023
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+MacBook Pro Mockups
+December 2022
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Veronika Bochkareva
+3D Artist
+iPhone 14 Pro Mockups
+November 2022
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Veronika Bochkareva
+3D Artist
+Holographic Abstract 3D Backgrounds
+November 2022
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Veronika Bochkareva
+3D Artist
+Egor Mishin
+Free Halloween 3D illustrations (2.0)
+October 2022
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Veronika Bochkareva
+3D Artist
+Big Sale
+October 2022
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Veronika Bochkareva
+3D Artist
+Abstract 3d illustrations
+August 2022
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Veronika Bochkareva
+3D Artist
+Inflatable 3d alphabet
+August 2022
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Veronika Bochkareva
+3D Artist
+Space 3d illustration
+May 2022
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Retro 3d illustrations
+April 2022
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Humans 3D Characters V3.0
+January 2022
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+3D Charts
+December 2021
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Free Christmas 3D Illustrations
+November 2021
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Free 3D Halloween Illustrations
+October 2021
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Kukla 3d icon kit (v2.0)
+October 2021
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Security 3D Icons
+August 2021
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Emoji
+July 2021
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+LOOPS
+February 2021
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Humans
+October 2020
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin
+Kukla kit
+June 2020
+Follow All
+Anton Mishin
+Co-founder at Wannathis.one
+Egor Mishin</t>
+  </si>
+  <si>
     <t>Read Me Aloud</t>
   </si>
   <si>
@@ -297,6 +791,13 @@
     <t>https://www.producthunt.com/posts/read-me-aloud?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Read Me Aloud
+January 2023
+Follow All
+Davide Benini
+Maker of Menu Plan and Read me Aloud</t>
+  </si>
+  <si>
     <t>DeepReview</t>
   </si>
   <si>
@@ -306,6 +807,14 @@
     <t>https://www.producthunt.com/posts/deepreview?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>DeepReview
+January 2023
+Follow All
+Horia Coman
+Software engineer at Stack Overflow
+Liviu Coman</t>
+  </si>
+  <si>
     <t>Git Assistant</t>
   </si>
   <si>
@@ -315,6 +824,13 @@
     <t>https://www.producthunt.com/posts/git-assistant?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Git Assistant
+January 2023
+Follow All
+Andrew Kondelin
+Developer, improving my marketing skills</t>
+  </si>
+  <si>
     <t>Anagramish</t>
   </si>
   <si>
@@ -324,6 +840,12 @@
     <t>https://www.producthunt.com/posts/anagramish?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Anagramish
+January 2023
+Follow All
+Evan Haveman</t>
+  </si>
+  <si>
     <t>EffectiveGPT</t>
   </si>
   <si>
@@ -333,6 +855,13 @@
     <t>https://www.producthunt.com/posts/effectivegpt?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>EffectiveGPT
+January 2023
+Follow All
+Recurrsed
+I build random useless stuff...</t>
+  </si>
+  <si>
     <t>Bubbly</t>
   </si>
   <si>
@@ -342,6 +871,13 @@
     <t>https://www.producthunt.com/posts/bubbly-3?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Bubbly
+January 2023
+Follow All
+Andy
+Bubbly Team</t>
+  </si>
+  <si>
     <t>Twitter for Noobs</t>
   </si>
   <si>
@@ -360,6 +896,13 @@
     <t>https://www.producthunt.com/posts/chatgenie?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>ChatGenie
+January 2023
+Follow All
+Patrick
+26 | Crafting stuff</t>
+  </si>
+  <si>
     <t>Recipes By AI</t>
   </si>
   <si>
@@ -369,6 +912,13 @@
     <t>https://www.producthunt.com/posts/recipes-by-ai-2?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Recipes By AI
+January 2023
+Follow All
+Lewis Crutch
+Building Content Websites and AI Tools</t>
+  </si>
+  <si>
     <t>wallaroo</t>
   </si>
   <si>
@@ -378,6 +928,15 @@
     <t>https://www.producthunt.com/posts/wallaroo?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>wallaroo
+January 2023
+Follow All
+Von Glitschka
+I create design and live near Bigfoot.
+Craig Hockenberry
+I GET PAID TO TYPE</t>
+  </si>
+  <si>
     <t>Møbel</t>
   </si>
   <si>
@@ -387,6 +946,13 @@
     <t>https://www.producthunt.com/posts/mobel-2?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Møbel
+January 2023
+Follow All
+Pontus Aurdal
+IoT, AWS, serverless, event-driven.</t>
+  </si>
+  <si>
     <t>Atomic</t>
   </si>
   <si>
@@ -396,6 +962,13 @@
     <t>https://www.producthunt.com/posts/atomic-4?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Atomic
+January 2023
+Follow All
+Rish
+Indiehacker running a solo biz</t>
+  </si>
+  <si>
     <t>Loti</t>
   </si>
   <si>
@@ -405,6 +978,17 @@
     <t>https://www.producthunt.com/posts/loti-2?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Loti
+January 2023
+Follow All
+Luke Arrigoni
+Founder of multiple AI companies.
+Rebekah Arrigoni
+Co-founder and CEO of Loti
+Hirak Chhatbar
+Co-founder and Chief Technology Officer</t>
+  </si>
+  <si>
     <t>Wifi QR Code</t>
   </si>
   <si>
@@ -414,6 +998,13 @@
     <t>https://www.producthunt.com/posts/wifi-qr-code?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Wifi QR Code
+January 2023
+Follow All
+Max Sommer
+Web Developer. Curious person.</t>
+  </si>
+  <si>
     <t>ChatGPT Prompts</t>
   </si>
   <si>
@@ -423,6 +1014,12 @@
     <t>https://www.producthunt.com/posts/chatgpt-prompts?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>ChatGPT Prompts
+January 2023
+Follow All
+Adrien</t>
+  </si>
+  <si>
     <t>Text2SQL.AI</t>
   </si>
   <si>
@@ -432,6 +1029,13 @@
     <t>https://www.producthunt.com/posts/text2sql-ai?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Text2SQL.AI
+January 2023
+Follow All
+Gary Miklos
+Bootstrapped solopreneur.</t>
+  </si>
+  <si>
     <t>Jobs Scout</t>
   </si>
   <si>
@@ -441,6 +1045,13 @@
     <t>https://www.producthunt.com/posts/jobs-scout?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Jobs Scout
+January 2023
+Follow All
+Sasi
+I like to build stuff!</t>
+  </si>
+  <si>
     <t>What Word Is That?</t>
   </si>
   <si>
@@ -450,6 +1061,13 @@
     <t>https://www.producthunt.com/posts/what-word-is-that?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>What Word Is That?
+January 2023
+Follow All
+Michael Li
+Software Engineer</t>
+  </si>
+  <si>
     <t>Pencil AI</t>
   </si>
   <si>
@@ -459,6 +1077,13 @@
     <t>https://www.producthunt.com/posts/pencil-ai?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Pencil AI
+January 2023
+Follow All
+Arafat Akata
+A software developer</t>
+  </si>
+  <si>
     <t>Vucac</t>
   </si>
   <si>
@@ -468,6 +1093,13 @@
     <t>https://www.producthunt.com/posts/vucac?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Vucac
+January 2023
+Follow All
+Vaux Calvert
+A board</t>
+  </si>
+  <si>
     <t>Circle</t>
   </si>
   <si>
@@ -477,6 +1109,13 @@
     <t>https://www.producthunt.com/posts/circle-98339679-23ac-4593-a2f8-b9b63a697717?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Circle
+January 2023
+Follow All
+Manuel Pirhofer
+👋 Hi, I am Manuel</t>
+  </si>
+  <si>
     <t>Time Boxing Planner</t>
   </si>
   <si>
@@ -486,6 +1125,13 @@
     <t>https://www.producthunt.com/posts/time-boxing-planner?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Time Boxing Planner
+January 2023
+Follow All
+Sourabh
+The Notion Buddy</t>
+  </si>
+  <si>
     <t>Mirror</t>
   </si>
   <si>
@@ -504,6 +1150,13 @@
     <t>https://www.producthunt.com/posts/notion-ultimate-life-planner?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Notion Ultimate Life Planner
+January 2023
+Follow All
+Modest Mitkus
+Solopreneur</t>
+  </si>
+  <si>
     <t>AutoPay</t>
   </si>
   <si>
@@ -513,6 +1166,14 @@
     <t>https://www.producthunt.com/posts/autopay?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>AutoPay
+January 2023
+Follow All
+Deep Sheth
+Solving problems for content creators
+Priyanshu Panda</t>
+  </si>
+  <si>
     <t>IdeaTank</t>
   </si>
   <si>
@@ -522,6 +1183,15 @@
     <t>https://www.producthunt.com/posts/ideatank?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>IdeaTank
+January 2023
+Follow All
+Arpit
+Just Another Person Seeking Problems
+Aakash Kumar
+Building IdeaTank</t>
+  </si>
+  <si>
     <t>Vikara</t>
   </si>
   <si>
@@ -531,6 +1201,13 @@
     <t>https://www.producthunt.com/posts/vikara?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Vikara
+January 2023
+Follow All
+Pravin Halady
+Building Vikara, a chatbot nutritionist</t>
+  </si>
+  <si>
     <t>Cron Jobs Expert</t>
   </si>
   <si>
@@ -540,6 +1217,13 @@
     <t>https://www.producthunt.com/posts/cron-jobs-expert?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Cron Jobs Expert
+January 2023
+Follow All
+Daniel Nikulshyn
+Senior 👨‍💻</t>
+  </si>
+  <si>
     <t>Optic Weather</t>
   </si>
   <si>
@@ -549,6 +1233,12 @@
     <t>https://www.producthunt.com/posts/optic-weather?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Optic Weather
+January 2023
+Follow All
+Tonye</t>
+  </si>
+  <si>
     <t>Tab Manager Auto</t>
   </si>
   <si>
@@ -558,6 +1248,13 @@
     <t>https://www.producthunt.com/posts/tab-manager-auto?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Tab Manager Auto
+January 2023
+Follow All
+Kevin Wang
+Building chrome extensions.</t>
+  </si>
+  <si>
     <t>Plum Notes</t>
   </si>
   <si>
@@ -567,6 +1264,13 @@
     <t>https://www.producthunt.com/posts/plum-notes?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Plum Notes
+January 2023
+Follow All
+Ian Mora
+Cretor of plum notes app.</t>
+  </si>
+  <si>
     <t>mock.qa</t>
   </si>
   <si>
@@ -576,6 +1280,17 @@
     <t>https://www.producthunt.com/posts/mock-qa?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>mock.qa
+January 2023
+Follow All
+Evgeniy Kosjakov
+Senior Test Automation Engineer
+Victor Vorobyev
+Software Engineer
+Vladimir Solovev
+Software Engineer</t>
+  </si>
+  <si>
     <t>OmniWork</t>
   </si>
   <si>
@@ -585,6 +1300,19 @@
     <t>https://www.producthunt.com/posts/omniwork-2?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>OmniWork
+January 2023
+Follow All
+Flavio
+Solution Architect
+Sohrab Tellaie
+I'm Sohrab. CEO &amp; Co-founder of OmniWork
+Lawrence Chan
+Making Great Products Greater
+Mazdak Sorosh
+Beezhan</t>
+  </si>
+  <si>
     <t>Dookey Dash</t>
   </si>
   <si>
@@ -603,6 +1331,13 @@
     <t>https://www.producthunt.com/posts/calendar-query?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Calendar Query
+January 2023
+Follow All
+Devon Bradley
+Shipping software products 🚀</t>
+  </si>
+  <si>
     <t>Furmasterpiece Pet Avatar Creator</t>
   </si>
   <si>
@@ -612,6 +1347,13 @@
     <t>https://www.producthunt.com/posts/furmasterpiece-pet-avatar-creator?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Furmasterpiece Pet Avatar Creator
+January 2023
+Follow All
+Rando Tkatsenko
+Building cool stuff with Unity- VR, AI.</t>
+  </si>
+  <si>
     <t>GiftBot: Love Edition</t>
   </si>
   <si>
@@ -621,6 +1363,18 @@
     <t>https://www.producthunt.com/posts/giftbot-love-edition?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>GiftBot: Love Edition
+January 2023
+Follow All
+Anish Thite
+Master procrastinator
+GiftBot
+December 2022
+Follow All
+Anish Thite
+Master procrastinator</t>
+  </si>
+  <si>
     <t>Internet Is Beautiful</t>
   </si>
   <si>
@@ -630,6 +1384,13 @@
     <t>https://www.producthunt.com/posts/internet-is-beautiful?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Internet Is Beautiful
+January 2023
+Follow All
+Jaisal Rathee
+Building www.startups.fyi 🦄</t>
+  </si>
+  <si>
     <t>WorkHub Connect for Mobile</t>
   </si>
   <si>
@@ -639,6 +1400,56 @@
     <t>https://www.producthunt.com/posts/workhub-connect-for-mobile?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>WorkHub Connect for Mobile
+January 2023
+Follow All
+Hamza Afzal Butt
+B2B SaaS Growth Marketing Consultant
+Qudsia Ali
+Director at WorkHub
+Sidra Ali
+Founder @Vadoreu
+Noshaid Ali
+Senior Software Engineer
+Bilal Anwar
+Mobile App Developer @ Workhub
+Aqsa Sajjad
+Digital Marketing
+Show all 8 makers
+WorkHub eSignature
+November 2022
+Follow All
+Qudsia Ali
+Director at WorkHub
+WorkHub Scheduling
+September 2022
+Follow All
+Qudsia Ali
+Director at WorkHub
+WorkHub
+September 2022
+Follow All
+Qudsia Ali
+Director at WorkHub
+WorkHub Spaces
+August 2022
+Follow All
+Qudsia Ali
+Director at WorkHub
+BRAVO!
+July 2022
+Follow All
+Qudsia Ali
+Director at WorkHub
+WorkHub Connect
+April 2022
+Follow All
+Nabeel Amir
+I am the Product Owner @ WorkHub
+Ali Naqi Shaheen
+Entrepreneur, Angel Investor</t>
+  </si>
+  <si>
     <t>The Help Center Academy</t>
   </si>
   <si>
@@ -648,6 +1459,13 @@
     <t>https://www.producthunt.com/posts/the-help-center-academy?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>The Help Center Academy
+January 2023
+Follow All
+Dominik Sobe
+⚡Indie Hacker building interweb products</t>
+  </si>
+  <si>
     <t>Makelog</t>
   </si>
   <si>
@@ -657,6 +1475,20 @@
     <t>https://www.producthunt.com/posts/makelog?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Makelog
+January 2023
+Follow All
+JJ Nguyen
+Briton Baker
+Product Designer
+Julio Farah
+f
+Jacob Hubbard
+building makelog
+Logan Liffick
+Senior Designer at DigitalOcean</t>
+  </si>
+  <si>
     <t>Pitchdeck Challenge</t>
   </si>
   <si>
@@ -666,6 +1498,13 @@
     <t>https://www.producthunt.com/posts/pitchdeck-challenge?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Pitchdeck Challenge
+January 2023
+Follow All
+Sebastian Janus - derStartupCFO
+Founder &amp; Serial Entrepreneur</t>
+  </si>
+  <si>
     <t>Inside AI</t>
   </si>
   <si>
@@ -675,6 +1514,13 @@
     <t>https://www.producthunt.com/posts/inside-ai?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Inside AI
+January 2023
+Follow All
+Jan Sulek
+AI Newsletter - insideai.co</t>
+  </si>
+  <si>
     <t>Product Launch AI</t>
   </si>
   <si>
@@ -684,6 +1530,13 @@
     <t>https://www.producthunt.com/posts/product-launch-ai?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Product Launch AI
+January 2023
+Follow All
+Adithya Shreshti
+Startup Launch &amp; NoCode Consultant</t>
+  </si>
+  <si>
     <t>MusicLM by Google</t>
   </si>
   <si>
@@ -702,6 +1555,13 @@
     <t>https://www.producthunt.com/posts/casper-5?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Casper
+January 2023
+Follow All
+Johan
+Building and thinking AI stuff</t>
+  </si>
+  <si>
     <t>Social Media Manager</t>
   </si>
   <si>
@@ -711,6 +1571,13 @@
     <t>https://www.producthunt.com/posts/social-media-manager-2?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Social Media Manager
+January 2023
+Follow All
+Brian
+Product Designer &amp; Notion Creator</t>
+  </si>
+  <si>
     <t>dbt-infer</t>
   </si>
   <si>
@@ -720,6 +1587,15 @@
     <t>https://www.producthunt.com/posts/dbt-infer?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>dbt-infer
+January 2023
+Follow All
+Ryan Garland
+Hello!
+Erik Mathiesen-Dreyfus
+Founder@Infer</t>
+  </si>
+  <si>
     <t>The Guest Posts App</t>
   </si>
   <si>
@@ -729,6 +1605,13 @@
     <t>https://www.producthunt.com/posts/the-guest-posts-app?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>The Guest Posts App
+January 2023
+Follow All
+Siddharth Verma
+SAAS Consultant | Startups | AI/NLP</t>
+  </si>
+  <si>
     <t>hai Infusions Smart Showerhead</t>
   </si>
   <si>
@@ -738,6 +1621,24 @@
     <t>https://www.producthunt.com/posts/hai-infusions-smart-showerhead?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>hai Infusions Smart Showerhead
+January 2023
+Follow All
+Leah Stigile
+Co-founder &amp; CEO
+Gina Oh
+Cofounder
+Kate Starr
+VP and storyteller of amazing showers.
+Monika Markovinovic
+content person. loves the internet.
+Leonard Brody
+CEO
+Madi Fisk
+Intern @hai
+Show all 7 makers</t>
+  </si>
+  <si>
     <t>Welma</t>
   </si>
   <si>
@@ -747,6 +1648,13 @@
     <t>https://www.producthunt.com/posts/welma?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
+    <t>Welma
+January 2023
+Follow All
+Mighil
+globe-earther and schnauzer enthusiast</t>
+  </si>
+  <si>
     <t>Followup Fish</t>
   </si>
   <si>
@@ -756,7 +1664,11 @@
     <t>https://www.producthunt.com/posts/followup-fish?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376802</t>
+    <t>Followup Fish
+January 2023
+Follow All
+Marc Köhlbrugge
+Founder of BetaList</t>
   </si>
   <si>
     <t>Extractify</t>
@@ -768,7 +1680,11 @@
     <t>https://www.producthunt.com/posts/extractify?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>375422</t>
+    <t>Extractify
+January 2023
+Follow All
+Ahsan Shahid
+Builder</t>
   </si>
   <si>
     <t>Spot a Bot</t>
@@ -780,7 +1696,17 @@
     <t>https://www.producthunt.com/posts/spot-a-bot?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376669</t>
+    <t>Spot a Bot
+January 2023
+Follow All
+Nicolas Graf
+Heavy web consumer and creator.
+Kevin Harizaj
+Developer
+Lena Heiglauer
+Developer @ Spot A Bot
+Daniela Dottolo
+Web Development student from Austria 🌈</t>
   </si>
   <si>
     <t>Semantic AI</t>
@@ -792,7 +1718,11 @@
     <t>https://www.producthunt.com/posts/semantic-ai?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376685</t>
+    <t>Semantic AI
+January 2023
+Follow All
+Amu
+Founder of Sentiment</t>
   </si>
   <si>
     <t>MailGPT</t>
@@ -804,7 +1734,11 @@
     <t>https://www.producthunt.com/posts/mailgpt?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376717</t>
+    <t>MailGPT
+January 2023
+Follow All
+Sourav Kumar Pradhan
+Developer</t>
   </si>
   <si>
     <t>Multichain Playbook</t>
@@ -816,7 +1750,22 @@
     <t>https://www.producthunt.com/posts/multichain-playbook?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376640</t>
+    <t>Multichain Playbook
+January 2023
+Follow All
+Dinesh Kruplani
+Growth &amp; Marketing at Dehidden
+Ramees P S
+Product | Growth | Crypto
+Sangeet Muralidhar
+building stuff
+Sahil Pednekar
+Product Designer, NFT Artist
+Avinash Kumar
+Product Designer
+Harikrishnaraj
+Project Manager
+Show all 7 makers</t>
   </si>
   <si>
     <t>Oura for Apple Watch</t>
@@ -828,7 +1777,13 @@
     <t>https://www.producthunt.com/posts/oura-for-apple-watch?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376756</t>
+    <t>Oura for Apple Watch
+January 2023
+Follow All
+Jason Russell
+Director of Product at Oura Ring
+Petteri Lahtela
+CEO, Co-Founder at ŌURA</t>
   </si>
   <si>
     <t>ciphergoat</t>
@@ -840,7 +1795,15 @@
     <t>https://www.producthunt.com/posts/ciphergoat?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376757</t>
+    <t>ciphergoat
+January 2023
+Follow All
+Aaron Pardes
+Building things with code
+Danilo Bandovic
+Lawyer with a business mindset.
+Ron Edgar
+CEO &amp; Co-founder | Genius Goat Labs Inc.</t>
   </si>
   <si>
     <t>SULO-Y</t>
@@ -852,9 +1815,6 @@
     <t>https://www.producthunt.com/posts/sulo-y?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376750</t>
-  </si>
-  <si>
     <t>SpicyHR</t>
   </si>
   <si>
@@ -864,7 +1824,13 @@
     <t>https://www.producthunt.com/posts/spicyhr?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376841</t>
+    <t>SpicyHR
+January 2023
+Follow All
+Ali Mir
+Co-founder at Spicy.hr
+Meisam Movassat
+Co-founder at Vasona; simplify hiring.</t>
   </si>
   <si>
     <t>Shell GPT</t>
@@ -876,9 +1842,6 @@
     <t>https://www.producthunt.com/posts/shell-gpt?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376758</t>
-  </si>
-  <si>
     <t>Lightness</t>
   </si>
   <si>
@@ -888,7 +1851,11 @@
     <t>https://www.producthunt.com/posts/lightness?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376855</t>
+    <t>Lightness
+January 2023
+Follow All
+Stefano Ippolito Gitto
+Founder of Lightness</t>
   </si>
   <si>
     <t>Moodlody</t>
@@ -900,7 +1867,11 @@
     <t>https://www.producthunt.com/posts/moodlody?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376875</t>
+    <t>Moodlody
+January 2023
+Follow All
+Dream.Chayutpong
+Front-End Developer.</t>
   </si>
   <si>
     <t>Todidlist</t>
@@ -912,7 +1883,10 @@
     <t>https://www.producthunt.com/posts/todidlist?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376434</t>
+    <t>Todidlist
+January 2023
+Follow All
+Patrick Tran</t>
   </si>
   <si>
     <t>Ask by Slite</t>
@@ -924,7 +1898,124 @@
     <t>https://www.producthunt.com/posts/ask-by-slite?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>375110</t>
+    <t>Ask by Slite
+January 2023
+Follow All
+Christophe Pasquier
+Founder @ Slite
+Jon McCullough
+Product Marketing at Slite
+Pierre Renaudin
+Sliter
+Fadeelah Al-horaibi
+Head of Product @Slite
+Ani Cordani
+Clara Rua
+Product designer
+Show all 22 makers
+Slite Discussions
+June 2022
+Follow All
+Ani Cordani
+Jon McCullough
+Product Marketing at Slite
+Christophe Pasquier
+Founder @ Slite
+Pierre Renaudin
+Sliter
+Clara Rua
+Product designer
+Brieuc Sebillotte
+Show all 14 makers
+Slite + Excalidraw
+February 2021
+Follow All
+Christophe Pasquier
+Founder @ Slite
+Antoine Duban
+Slite 2.0
+October 2020
+Follow All
+Clara Rua
+Product designer
+michael bartlett
+Christophe Pasquier
+Founder @ Slite
+Pierre Renaudin
+Sliter
+Draft by Slite
+July 2020
+Follow All
+Arnaud Rinquin
+Laure Albouy
+marketing @ bonsai
+Charley D.
+Clara Rua
+Product designer
+Lead by Writing
+September 2019
+Follow All
+Rob McMackin
+Product designer @ Slite
+Laure Albouy
+marketing @ bonsai
+Christophe Pasquier
+Founder @ Slite
+Startup Bibles
+May 2019
+Follow All
+Laure Albouy
+marketing @ bonsai
+Clara Rua
+Product designer
+Adrien Taravant
+Employee onboarding checklist
+February 2019
+Follow All
+Laure Albouy
+marketing @ bonsai
+Adrien Taravant
+Clara Rua
+Product designer
+Slite for Mobile
+December 2018
+Follow All
+Clara Rua
+Product designer
+Guillaume Morin
+Lead Mobile engineer @slitehq 👨‍💻📱⚛️
+Christophe Pasquier
+Founder @ Slite
+Charley D.
+Pierre Renaudin
+Sliter
+Arnaud Rinquin
+Templates by Slite
+January 2018
+Follow All
+Alexandre Gaudencio
+Spaceship launcher @ Slite
+Clara Rua
+Product designer
+Clément Rucheton
+Brieuc Sebillotte
+Arnaud Rinquin
+Antoine Duban
+Show all 9 makers
+Slite
+October 2017
+Follow All
+Laure Albouy
+marketing @ bonsai
+Brieuc Sebillotte
+Arnaud Rinquin
+Pierre Renaudin
+Sliter
+Christophe Pasquier
+Founder @ Slite
+Rob McMackin
+Product designer @ Slite
+Show all 14 makers</t>
   </si>
   <si>
     <t>Charlie</t>
@@ -936,7 +2027,20 @@
     <t>https://www.producthunt.com/posts/charlie-6?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>374952</t>
+    <t>Charlie
+January 2023
+Follow All
+Brennan Woodruff
+Finance guy gone AI Product Developer
+Kostas Hatalis
+CEO of GoCharlie.ai
+Despina Christou
+.
+Charlie 2.0
+September 2022
+Follow All
+Brennan Woodruff
+Finance guy gone AI Product Developer</t>
   </si>
   <si>
     <t>NeevaAI</t>
@@ -948,7 +2052,38 @@
     <t>https://www.producthunt.com/posts/neevaai?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376466</t>
+    <t>NeevaAI
+January 2023
+Follow All
+Hwi Lee
+Head of Design @Neeva
+Yusuf Ozuysal
+Mobile @Neeva
+Seth Li
+Growth @ Neeva
+Jiwoong Lee
+UX designer, Neeva
+Cooper LaRhette
+SWE @ Neeva
+Rajhans Samdani
+Head of Machine Learning, Neeva
+Show all 10 makers
+Neeva
+July 2021
+Follow All
+Seth Li
+Growth @ Neeva
+Edmund Loo
+edmundloo.com
+Darin Fisher
+browser builder @neeva
+Sridhar Ramaswamy
+@neeva Co-Founder Ex-@Google SVP Ads
+Rachel Cheng
+Product Designer
+Anton Borzov
+Product Design. Formerly @WhatsApp.
+Show all 8 makers</t>
   </si>
   <si>
     <t>WritingMate.ai</t>
@@ -960,7 +2095,11 @@
     <t>https://www.producthunt.com/posts/writingmate-ai?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>375784</t>
+    <t>WritingMate.ai
+January 2023
+Follow All
+Alexander Nevedovsky
+Artem Vysotsky</t>
   </si>
   <si>
     <t>Conektto API-First Design Studio</t>
@@ -972,7 +2111,15 @@
     <t>https://www.producthunt.com/posts/conektto-api-first-design-studio?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>375864</t>
+    <t>Conektto API-First Design Studio
+January 2023
+Follow All
+Ram Sathia
+Automation obsessed technologist
+Amol Dewhare
+Founder &amp; CEO of Conektto
+Madhu V Swamy
+Technopreneur building digital products</t>
   </si>
   <si>
     <t>Figma to WordPress Beta</t>
@@ -984,7 +2131,39 @@
     <t>https://www.producthunt.com/posts/figma-to-wordpress-beta?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
   </si>
   <si>
-    <t>376506</t>
+    <t>Figma to WordPress Beta
+January 2023
+Follow All
+Alfonso García Frey
+Building nextgen design technology
+Cédric Legendre
+Maurício
+Software Dev, gamer and guitar player
+Ali mot
+Software engineer
+Ilyes El ayeb
+software engineer
+Sanine Moreira
+Show all 7 makers
+WordPress for Adobe XD
+September 2022
+Follow All
+Alfonso García Frey
+Building nextgen design technology
+Cédric Legendre
+Maurício
+Software Dev, gamer and guitar player
+Ali mot
+Software engineer
+Ilyes El ayeb
+software engineer
+Sanine Moreira
+Show all 7 makers
+Yotako
+December 2018
+Follow All
+Alfonso García Frey
+Building nextgen design technology</t>
   </si>
   <si>
     <t>Alt Sprints</t>
@@ -994,6 +2173,30 @@
   </si>
   <si>
     <t>https://www.producthunt.com/posts/alt-sprints?utm_campaign=producthunt-api&amp;utm_medium=api-v2&amp;utm_source=Application%3A+test2+%28ID%3A+95747%29</t>
+  </si>
+  <si>
+    <t>NoLoCo Stack
+February 2023
+Follow All
+Ali Haider
+Building a venture studio
+Ahsan Asghar
+Product Manager
+Ahsan Sohail
+Venture Builder @ Alt Sprints
+Alt Sprints
+January 2023
+Follow All
+Yetunde Lopez
+Product designer
+Umair Abdullah
+Founder, digital nomad and storyteller.
+Ahsan Asghar
+Product Manager
+Ali Haider
+Building a venture studio
+Ahsan Sohail
+Venture Builder @ Alt Sprints</t>
   </si>
 </sst>
 </file>
@@ -1049,10 +2252,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1356,22 +2562,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="49" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="6" max="6" width="72.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1387,1705 +2594,1987 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>375989</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>1022</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>377157</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>466</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>376810</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E4">
         <v>370</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>376335</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>251</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>376853</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E6">
         <v>261</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>377091</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>271</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>377162</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E8">
         <v>232</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="360" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>376934</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E9">
         <v>272</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>377110</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E10">
         <v>206</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>377104</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E11">
         <v>160</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>376474</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="E12">
         <v>138</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>377113</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E13">
         <v>120</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>376809</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E14">
         <v>117</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>377095</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="E15">
         <v>133</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>375586</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="E16">
         <v>123</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>377115</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="E17">
         <v>89</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>375401</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="E18">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>377208</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="E19">
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>376579</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="E20">
         <v>76</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="360" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>377154</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E21">
         <v>66</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>377195</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="D22" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E22">
         <v>60</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>377087</v>
       </c>
       <c r="B23" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="E23">
         <v>56</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>377100</v>
       </c>
       <c r="B24" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="E24">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>376954</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="E25">
         <v>44</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>377071</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="E26">
         <v>54</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>376994</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E27">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>377245</v>
       </c>
       <c r="B28" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="E28">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>376612</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
       <c r="E29">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>373387</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="E30">
         <v>36</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>377229</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="E31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>377177</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="C32" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="E32">
         <v>26</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>377160</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>130</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="E33">
         <v>28</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>377249</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="E34">
         <v>26</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>377231</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>137</v>
       </c>
       <c r="C35" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
-        <v>106</v>
+        <v>139</v>
       </c>
       <c r="E35">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>374958</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="D36" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="E36">
         <v>331</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>376775</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="C37" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
       <c r="D37" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
       <c r="E37">
         <v>248</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>376839</v>
       </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="C38" t="s">
-        <v>114</v>
+        <v>149</v>
       </c>
       <c r="D38" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="E38">
         <v>195</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>377000</v>
       </c>
       <c r="B39" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="C39" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="D39" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="E39">
         <v>151</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>376815</v>
       </c>
       <c r="B40" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="C40" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="D40" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
       <c r="E40">
         <v>135</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>376741</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>160</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>161</v>
       </c>
       <c r="D41" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
       <c r="E41">
         <v>115</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>376414</v>
       </c>
       <c r="B42" t="s">
-        <v>125</v>
+        <v>164</v>
       </c>
       <c r="C42" t="s">
-        <v>126</v>
+        <v>165</v>
       </c>
       <c r="D42" t="s">
-        <v>127</v>
+        <v>166</v>
       </c>
       <c r="E42">
         <v>97</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>376977</v>
       </c>
       <c r="B43" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
       <c r="D43" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
       <c r="E43">
         <v>95</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>376966</v>
       </c>
       <c r="B44" t="s">
-        <v>131</v>
+        <v>172</v>
       </c>
       <c r="C44" t="s">
-        <v>132</v>
+        <v>173</v>
       </c>
       <c r="D44" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="E44">
         <v>96</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>373699</v>
       </c>
       <c r="B45" t="s">
-        <v>134</v>
+        <v>176</v>
       </c>
       <c r="C45" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="D45" t="s">
-        <v>136</v>
+        <v>178</v>
       </c>
       <c r="E45">
         <v>85</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>376878</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
+        <v>180</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
       <c r="D46" t="s">
-        <v>139</v>
+        <v>182</v>
       </c>
       <c r="E46">
         <v>90</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>377018</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
+        <v>184</v>
       </c>
       <c r="C47" t="s">
-        <v>141</v>
+        <v>185</v>
       </c>
       <c r="D47" t="s">
-        <v>142</v>
+        <v>186</v>
       </c>
       <c r="E47">
         <v>79</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>376967</v>
       </c>
       <c r="B48" t="s">
-        <v>143</v>
+        <v>188</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>189</v>
       </c>
       <c r="D48" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="E48">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>376951</v>
       </c>
       <c r="B49" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="C49" t="s">
-        <v>147</v>
+        <v>193</v>
       </c>
       <c r="D49" t="s">
-        <v>148</v>
+        <v>194</v>
       </c>
       <c r="E49">
         <v>50</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>376953</v>
       </c>
       <c r="B50" t="s">
-        <v>149</v>
+        <v>196</v>
       </c>
       <c r="C50" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
       <c r="D50" t="s">
-        <v>151</v>
+        <v>198</v>
       </c>
       <c r="E50">
         <v>42</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>376940</v>
       </c>
       <c r="B51" t="s">
-        <v>152</v>
+        <v>200</v>
       </c>
       <c r="C51" t="s">
-        <v>153</v>
+        <v>201</v>
       </c>
       <c r="D51" t="s">
-        <v>154</v>
+        <v>202</v>
       </c>
       <c r="E51">
         <v>249</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>376914</v>
       </c>
       <c r="B52" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="C52" t="s">
-        <v>156</v>
+        <v>205</v>
       </c>
       <c r="D52" t="s">
-        <v>157</v>
+        <v>206</v>
       </c>
       <c r="E52">
         <v>223</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>376834</v>
       </c>
       <c r="B53" t="s">
-        <v>158</v>
+        <v>207</v>
       </c>
       <c r="C53" t="s">
-        <v>159</v>
+        <v>208</v>
       </c>
       <c r="D53" t="s">
-        <v>160</v>
+        <v>209</v>
       </c>
       <c r="E53">
         <v>288</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>376645</v>
       </c>
       <c r="B54" t="s">
-        <v>161</v>
+        <v>211</v>
       </c>
       <c r="C54" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
       <c r="D54" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="E54">
         <v>167</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>376900</v>
       </c>
       <c r="B55" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
       <c r="C55" t="s">
-        <v>165</v>
+        <v>216</v>
       </c>
       <c r="D55" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="E55">
         <v>137</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>376921</v>
       </c>
       <c r="B56" t="s">
-        <v>167</v>
+        <v>219</v>
       </c>
       <c r="C56" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
       <c r="D56" t="s">
-        <v>169</v>
+        <v>221</v>
       </c>
       <c r="E56">
         <v>96</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>376949</v>
       </c>
       <c r="B57" t="s">
-        <v>170</v>
+        <v>223</v>
       </c>
       <c r="C57" t="s">
-        <v>171</v>
+        <v>224</v>
       </c>
       <c r="D57" t="s">
-        <v>172</v>
+        <v>225</v>
       </c>
       <c r="E57">
         <v>87</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>376916</v>
       </c>
       <c r="B58" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
       <c r="C58" t="s">
-        <v>174</v>
+        <v>228</v>
       </c>
       <c r="D58" t="s">
-        <v>175</v>
+        <v>229</v>
       </c>
       <c r="E58">
         <v>66</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>376917</v>
       </c>
       <c r="B59" t="s">
-        <v>176</v>
+        <v>231</v>
       </c>
       <c r="C59" t="s">
-        <v>177</v>
+        <v>232</v>
       </c>
       <c r="D59" t="s">
-        <v>178</v>
+        <v>233</v>
       </c>
       <c r="E59">
         <v>64</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>376633</v>
       </c>
       <c r="B60" t="s">
-        <v>179</v>
+        <v>235</v>
       </c>
       <c r="C60" t="s">
-        <v>180</v>
+        <v>236</v>
       </c>
       <c r="D60" t="s">
-        <v>181</v>
+        <v>237</v>
       </c>
       <c r="E60">
         <v>64</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>375646</v>
       </c>
       <c r="B61" t="s">
-        <v>182</v>
+        <v>239</v>
       </c>
       <c r="C61" t="s">
-        <v>183</v>
+        <v>240</v>
       </c>
       <c r="D61" t="s">
-        <v>184</v>
+        <v>241</v>
       </c>
       <c r="E61">
         <v>66</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>376886</v>
       </c>
       <c r="B62" t="s">
-        <v>185</v>
+        <v>243</v>
       </c>
       <c r="C62" t="s">
-        <v>186</v>
+        <v>244</v>
       </c>
       <c r="D62" t="s">
-        <v>187</v>
+        <v>245</v>
       </c>
       <c r="E62">
         <v>56</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>376929</v>
       </c>
       <c r="B63" t="s">
-        <v>188</v>
+        <v>247</v>
       </c>
       <c r="C63" t="s">
-        <v>189</v>
+        <v>248</v>
       </c>
       <c r="D63" t="s">
-        <v>190</v>
+        <v>249</v>
       </c>
       <c r="E63">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>376772</v>
       </c>
       <c r="B64" t="s">
-        <v>191</v>
+        <v>250</v>
       </c>
       <c r="C64" t="s">
-        <v>192</v>
+        <v>251</v>
       </c>
       <c r="D64" t="s">
-        <v>193</v>
+        <v>252</v>
       </c>
       <c r="E64">
         <v>41</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64" s="2" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>376743</v>
       </c>
       <c r="B65" t="s">
-        <v>194</v>
+        <v>254</v>
       </c>
       <c r="C65" t="s">
-        <v>195</v>
+        <v>255</v>
       </c>
       <c r="D65" t="s">
-        <v>196</v>
+        <v>256</v>
       </c>
       <c r="E65">
         <v>42</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>376937</v>
       </c>
       <c r="B66" t="s">
-        <v>197</v>
+        <v>258</v>
       </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>259</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>260</v>
       </c>
       <c r="E66">
         <v>40</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>376701</v>
       </c>
       <c r="B67" t="s">
-        <v>200</v>
+        <v>262</v>
       </c>
       <c r="C67" t="s">
-        <v>201</v>
+        <v>263</v>
       </c>
       <c r="D67" t="s">
-        <v>202</v>
+        <v>264</v>
       </c>
       <c r="E67">
         <v>747</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67" s="2" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>376690</v>
       </c>
       <c r="B68" t="s">
-        <v>203</v>
+        <v>266</v>
       </c>
       <c r="C68" t="s">
-        <v>204</v>
+        <v>267</v>
       </c>
       <c r="D68" t="s">
-        <v>205</v>
+        <v>268</v>
       </c>
       <c r="E68">
         <v>651</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68" s="2" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>376172</v>
       </c>
       <c r="B69" t="s">
-        <v>206</v>
+        <v>270</v>
       </c>
       <c r="C69" t="s">
-        <v>207</v>
+        <v>271</v>
       </c>
       <c r="D69" t="s">
-        <v>208</v>
+        <v>272</v>
       </c>
       <c r="E69">
         <v>332</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>376770</v>
       </c>
       <c r="B70" t="s">
-        <v>209</v>
+        <v>274</v>
       </c>
       <c r="C70" t="s">
-        <v>210</v>
+        <v>275</v>
       </c>
       <c r="D70" t="s">
-        <v>211</v>
+        <v>276</v>
       </c>
       <c r="E70">
         <v>286</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>375921</v>
       </c>
       <c r="B71" t="s">
-        <v>212</v>
+        <v>278</v>
       </c>
       <c r="C71" t="s">
-        <v>213</v>
+        <v>279</v>
       </c>
       <c r="D71" t="s">
-        <v>214</v>
+        <v>280</v>
       </c>
       <c r="E71">
         <v>269</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>376388</v>
       </c>
       <c r="B72" t="s">
-        <v>215</v>
+        <v>282</v>
       </c>
       <c r="C72" t="s">
-        <v>216</v>
+        <v>283</v>
       </c>
       <c r="D72" t="s">
-        <v>217</v>
+        <v>284</v>
       </c>
       <c r="E72">
         <v>402</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>376177</v>
       </c>
       <c r="B73" t="s">
-        <v>218</v>
+        <v>286</v>
       </c>
       <c r="C73" t="s">
-        <v>219</v>
+        <v>287</v>
       </c>
       <c r="D73" t="s">
-        <v>220</v>
+        <v>288</v>
       </c>
       <c r="E73">
         <v>218</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>376859</v>
       </c>
       <c r="B74" t="s">
-        <v>221</v>
+        <v>290</v>
       </c>
       <c r="C74" t="s">
-        <v>222</v>
+        <v>291</v>
       </c>
       <c r="D74" t="s">
-        <v>223</v>
+        <v>292</v>
       </c>
       <c r="E74">
         <v>190</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>376393</v>
       </c>
       <c r="B75" t="s">
-        <v>224</v>
+        <v>293</v>
       </c>
       <c r="C75" t="s">
-        <v>225</v>
+        <v>294</v>
       </c>
       <c r="D75" t="s">
-        <v>226</v>
+        <v>295</v>
       </c>
       <c r="E75">
         <v>200</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>376755</v>
       </c>
       <c r="B76" t="s">
-        <v>227</v>
+        <v>297</v>
       </c>
       <c r="C76" t="s">
-        <v>228</v>
+        <v>298</v>
       </c>
       <c r="D76" t="s">
-        <v>229</v>
+        <v>299</v>
       </c>
       <c r="E76">
         <v>94</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76" s="2" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>376125</v>
       </c>
       <c r="B77" t="s">
-        <v>230</v>
+        <v>301</v>
       </c>
       <c r="C77" t="s">
-        <v>231</v>
+        <v>302</v>
       </c>
       <c r="D77" t="s">
-        <v>232</v>
+        <v>303</v>
       </c>
       <c r="E77">
         <v>86</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>376565</v>
       </c>
       <c r="B78" t="s">
-        <v>233</v>
+        <v>305</v>
       </c>
       <c r="C78" t="s">
-        <v>234</v>
+        <v>306</v>
       </c>
       <c r="D78" t="s">
-        <v>235</v>
+        <v>307</v>
       </c>
       <c r="E78">
         <v>82</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78" s="2" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>376789</v>
       </c>
       <c r="B79" t="s">
-        <v>236</v>
+        <v>309</v>
       </c>
       <c r="C79" t="s">
-        <v>237</v>
+        <v>310</v>
       </c>
       <c r="D79" t="s">
-        <v>238</v>
+        <v>311</v>
       </c>
       <c r="E79">
         <v>209</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>376731</v>
       </c>
       <c r="B80" t="s">
-        <v>239</v>
+        <v>313</v>
       </c>
       <c r="C80" t="s">
-        <v>240</v>
+        <v>314</v>
       </c>
       <c r="D80" t="s">
-        <v>241</v>
+        <v>315</v>
       </c>
       <c r="E80">
         <v>75</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>376786</v>
       </c>
       <c r="B81" t="s">
-        <v>242</v>
+        <v>317</v>
       </c>
       <c r="C81" t="s">
-        <v>243</v>
+        <v>318</v>
       </c>
       <c r="D81" t="s">
-        <v>244</v>
+        <v>319</v>
       </c>
       <c r="E81">
         <v>67</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>245</v>
+      <c r="F81" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>376802</v>
       </c>
       <c r="B82" t="s">
-        <v>246</v>
+        <v>321</v>
       </c>
       <c r="C82" t="s">
-        <v>247</v>
+        <v>322</v>
       </c>
       <c r="D82" t="s">
-        <v>248</v>
+        <v>323</v>
       </c>
       <c r="E82">
         <v>64</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>249</v>
+      <c r="F82" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>375422</v>
       </c>
       <c r="B83" t="s">
-        <v>250</v>
+        <v>325</v>
       </c>
       <c r="C83" t="s">
-        <v>251</v>
+        <v>326</v>
       </c>
       <c r="D83" t="s">
-        <v>252</v>
+        <v>327</v>
       </c>
       <c r="E83">
         <v>77</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>253</v>
+      <c r="F83" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>376669</v>
       </c>
       <c r="B84" t="s">
-        <v>254</v>
+        <v>329</v>
       </c>
       <c r="C84" t="s">
-        <v>255</v>
+        <v>330</v>
       </c>
       <c r="D84" t="s">
-        <v>256</v>
+        <v>331</v>
       </c>
       <c r="E84">
         <v>52</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>257</v>
+      <c r="F84" s="2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>376685</v>
       </c>
       <c r="B85" t="s">
-        <v>258</v>
+        <v>333</v>
       </c>
       <c r="C85" t="s">
-        <v>259</v>
+        <v>334</v>
       </c>
       <c r="D85" t="s">
-        <v>260</v>
+        <v>335</v>
       </c>
       <c r="E85">
         <v>48</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>261</v>
+      <c r="F85" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>376717</v>
       </c>
       <c r="B86" t="s">
-        <v>262</v>
+        <v>337</v>
       </c>
       <c r="C86" t="s">
-        <v>263</v>
+        <v>338</v>
       </c>
       <c r="D86" t="s">
-        <v>264</v>
+        <v>339</v>
       </c>
       <c r="E86">
         <v>42</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>265</v>
+      <c r="F86" s="2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>376640</v>
       </c>
       <c r="B87" t="s">
-        <v>266</v>
+        <v>341</v>
       </c>
       <c r="C87" t="s">
-        <v>267</v>
+        <v>342</v>
       </c>
       <c r="D87" t="s">
-        <v>268</v>
+        <v>343</v>
       </c>
       <c r="E87">
         <v>34</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>269</v>
+      <c r="F87" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>376756</v>
       </c>
       <c r="B88" t="s">
-        <v>270</v>
+        <v>345</v>
       </c>
       <c r="C88" t="s">
-        <v>271</v>
+        <v>346</v>
       </c>
       <c r="D88" t="s">
-        <v>272</v>
+        <v>347</v>
       </c>
       <c r="E88">
         <v>54</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>273</v>
+      <c r="F88" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>376757</v>
       </c>
       <c r="B89" t="s">
-        <v>274</v>
+        <v>349</v>
       </c>
       <c r="C89" t="s">
-        <v>275</v>
+        <v>350</v>
       </c>
       <c r="D89" t="s">
-        <v>276</v>
+        <v>351</v>
       </c>
       <c r="E89">
         <v>21</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>277</v>
+    <row r="90" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>376750</v>
       </c>
       <c r="B90" t="s">
-        <v>278</v>
+        <v>352</v>
       </c>
       <c r="C90" t="s">
-        <v>279</v>
+        <v>353</v>
       </c>
       <c r="D90" t="s">
-        <v>280</v>
+        <v>354</v>
       </c>
       <c r="E90">
         <v>20</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>281</v>
+      <c r="F90" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>376841</v>
       </c>
       <c r="B91" t="s">
-        <v>282</v>
+        <v>356</v>
       </c>
       <c r="C91" t="s">
-        <v>283</v>
+        <v>357</v>
       </c>
       <c r="D91" t="s">
-        <v>284</v>
+        <v>358</v>
       </c>
       <c r="E91">
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>285</v>
+    <row r="92" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>376758</v>
       </c>
       <c r="B92" t="s">
-        <v>286</v>
+        <v>359</v>
       </c>
       <c r="C92" t="s">
-        <v>287</v>
+        <v>360</v>
       </c>
       <c r="D92" t="s">
-        <v>288</v>
+        <v>361</v>
       </c>
       <c r="E92">
         <v>20</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>289</v>
+      <c r="F92" s="2" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>376855</v>
       </c>
       <c r="B93" t="s">
-        <v>290</v>
+        <v>363</v>
       </c>
       <c r="C93" t="s">
-        <v>291</v>
+        <v>364</v>
       </c>
       <c r="D93" t="s">
-        <v>292</v>
+        <v>365</v>
       </c>
       <c r="E93">
         <v>20</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>293</v>
+      <c r="F93" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>376875</v>
       </c>
       <c r="B94" t="s">
-        <v>294</v>
+        <v>367</v>
       </c>
       <c r="C94" t="s">
-        <v>295</v>
+        <v>368</v>
       </c>
       <c r="D94" t="s">
-        <v>296</v>
+        <v>369</v>
       </c>
       <c r="E94">
         <v>18</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>297</v>
+      <c r="F94" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>376434</v>
       </c>
       <c r="B95" t="s">
-        <v>298</v>
+        <v>371</v>
       </c>
       <c r="C95" t="s">
-        <v>299</v>
+        <v>372</v>
       </c>
       <c r="D95" t="s">
-        <v>300</v>
+        <v>373</v>
       </c>
       <c r="E95">
         <v>906</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>301</v>
+      <c r="F95" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>375110</v>
       </c>
       <c r="B96" t="s">
-        <v>302</v>
+        <v>375</v>
       </c>
       <c r="C96" t="s">
-        <v>303</v>
+        <v>376</v>
       </c>
       <c r="D96" t="s">
-        <v>304</v>
+        <v>377</v>
       </c>
       <c r="E96">
         <v>974</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>305</v>
+      <c r="F96" s="2" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>374952</v>
       </c>
       <c r="B97" t="s">
-        <v>306</v>
+        <v>379</v>
       </c>
       <c r="C97" t="s">
-        <v>307</v>
+        <v>380</v>
       </c>
       <c r="D97" t="s">
-        <v>308</v>
+        <v>381</v>
       </c>
       <c r="E97">
         <v>1117</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>309</v>
+      <c r="F97" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>376466</v>
       </c>
       <c r="B98" t="s">
-        <v>310</v>
+        <v>383</v>
       </c>
       <c r="C98" t="s">
-        <v>311</v>
+        <v>384</v>
       </c>
       <c r="D98" t="s">
-        <v>312</v>
+        <v>385</v>
       </c>
       <c r="E98">
         <v>739</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>313</v>
+      <c r="F98" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>375784</v>
       </c>
       <c r="B99" t="s">
-        <v>314</v>
+        <v>387</v>
       </c>
       <c r="C99" t="s">
-        <v>315</v>
+        <v>388</v>
       </c>
       <c r="D99" t="s">
-        <v>316</v>
+        <v>389</v>
       </c>
       <c r="E99">
         <v>541</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>317</v>
+      <c r="F99" s="2" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>375864</v>
       </c>
       <c r="B100" t="s">
-        <v>318</v>
+        <v>391</v>
       </c>
       <c r="C100" t="s">
-        <v>319</v>
+        <v>392</v>
       </c>
       <c r="D100" t="s">
-        <v>320</v>
+        <v>393</v>
       </c>
       <c r="E100">
         <v>462</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>321</v>
+      <c r="F100" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="330" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>376506</v>
       </c>
       <c r="B101" t="s">
-        <v>322</v>
+        <v>395</v>
       </c>
       <c r="C101" t="s">
-        <v>323</v>
+        <v>396</v>
       </c>
       <c r="D101" t="s">
-        <v>324</v>
+        <v>397</v>
       </c>
       <c r="E101">
         <v>295</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>